<commit_message>
Update RBC birth and death table.xlsx
</commit_message>
<xml_diff>
--- a/final_files/Manuscript/RBC birth and death table.xlsx
+++ b/final_files/Manuscript/RBC birth and death table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinepeters/Documents/GitHub/bdd/nw11_hier/final_files/Manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557A579B-E80A-3440-BD78-F576EAABBBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB98E9DC-9F08-5E47-9E77-B1FD15AD7815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15380" windowHeight="16640" xr2:uid="{4F3A513E-9F4E-CE40-9EA1-F3B9E1C88D22}"/>
+    <workbookView xWindow="7000" yWindow="740" windowWidth="38400" windowHeight="16680" xr2:uid="{4F3A513E-9F4E-CE40-9EA1-F3B9E1C88D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Birth</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Gravenor</t>
   </si>
   <si>
-    <t>No destruction of uninfected erythrocytes</t>
-  </si>
-  <si>
     <t>Constant production of erythrocytes</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>Constant input b</t>
   </si>
   <si>
-    <t xml:space="preserve">Mass action mu*S removal of susceptible RBC capturing aging; no removal of pRBCs via immunity; include linear mortaliyt of uRBCs to capture haemolytic anaemia </t>
-  </si>
-  <si>
     <t>RBC source has own ODE, with maximum rate of production; RBC production regulated by rate of loss of RBCs by means of normal sensecence or infection</t>
   </si>
   <si>
@@ -147,13 +141,37 @@
   </si>
   <si>
     <t>Changing rates of general RBC clearance and targeted pRBC clearance</t>
+  </si>
+  <si>
+    <t>Changing production of reticulocytes</t>
+  </si>
+  <si>
+    <t>Changing removal of general RBC clearance and targeted pRBC clearance</t>
+  </si>
+  <si>
+    <t>PHZ induced anaemia only</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No destruction of uninfected erythrocytes, just natural death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass action mu*S removal of susceptible RBC capturing aging; no removal of pRBCs via immunity; include linear mortaliy of uRBCs to capture haemolytic anaemia </t>
+  </si>
+  <si>
+    <t>Assume baseline replenishment is function of RBC density at homeostatic equilibrium Rc, times survival given background mortality during infection, given by mu_R''. Also have density-dependent replenishment.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +183,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -198,11 +223,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -225,15 +265,6 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -248,12 +279,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{512EF7A0-361A-DC4F-B624-92452F84085C}" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:C15" xr:uid="{512EF7A0-361A-DC4F-B624-92452F84085C}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0732922E-4F2C-C446-B0B1-D4CCF73F8367}" name="Paper" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{588C6740-F927-F741-BBA3-4BF25C0576C7}" name="Birth" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{F7EE33EA-15F7-BE40-822F-9567218BAF2A}" name="Death" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{512EF7A0-361A-DC4F-B624-92452F84085C}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D15" xr:uid="{512EF7A0-361A-DC4F-B624-92452F84085C}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0732922E-4F2C-C446-B0B1-D4CCF73F8367}" name="Paper" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{588C6740-F927-F741-BBA3-4BF25C0576C7}" name="Birth" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F7EE33EA-15F7-BE40-822F-9567218BAF2A}" name="Death" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5AA0AC3A-AA33-F744-A0AB-F57129B83A14}" name="Checked" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -556,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE48BA6F-8E2D-C149-A9FA-D6E5D65C0B39}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,9 +599,10 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="57.1640625" customWidth="1"/>
     <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="5" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -579,19 +612,23 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -601,90 +638,107 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -694,30 +748,48 @@
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>